<commit_message>
costing with LOC considerations
</commit_message>
<xml_diff>
--- a/Costing.xlsx
+++ b/Costing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganda\Documents\GitHub\Software-Engineering-Principles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AB335D-2357-4F1B-A634-592AC8D35512}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8676475C-47CA-47B5-83D6-ECA3609AD203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2251FB4-2332-4C94-8751-54E698B35F52}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Operation costs</t>
+  </si>
+  <si>
+    <t>Business VAT (20%)</t>
   </si>
 </sst>
 </file>
@@ -136,8 +139,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0">
-  <autoFilter ref="A1:C14" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C18B8DC8-D594-44F3-A9CB-962A72D8C656}" name="ID"/>
     <tableColumn id="2" xr3:uid="{AEE37500-31D3-4AF3-9ACB-22D32337DB85}" name="Feature"/>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6B2486-83C6-437F-9C90-794FF0F55BEE}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>600</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -488,7 +491,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>300</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -499,7 +502,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>300</v>
+        <v>510</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -532,7 +535,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>600</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -576,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>300</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -587,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>300</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -612,13 +615,25 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C2:C14)*0.2</f>
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <f>SUM(Table2[Cost])</f>
-        <v>9900</v>
+        <v>10908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
costing and documentation complete
</commit_message>
<xml_diff>
--- a/Costing.xlsx
+++ b/Costing.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganda\Documents\GitHub\Software-Engineering-Principles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8676475C-47CA-47B5-83D6-ECA3609AD203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9626E242-3F17-4F27-840E-A272D11A0E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2251FB4-2332-4C94-8751-54E698B35F52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2251FB4-2332-4C94-8751-54E698B35F52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -74,13 +79,7 @@
     <t>Moderation mode</t>
   </si>
   <si>
-    <t>Flagging system</t>
-  </si>
-  <si>
     <t>Website setup</t>
-  </si>
-  <si>
-    <t>Operation costs</t>
   </si>
   <si>
     <t>Business VAT (20%)</t>
@@ -139,8 +138,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{E0CE64BB-D476-43D8-A2C1-B6C52B6FDF17}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C18B8DC8-D594-44F3-A9CB-962A72D8C656}" name="ID"/>
     <tableColumn id="2" xr3:uid="{AEE37500-31D3-4AF3-9ACB-22D32337DB85}" name="Feature"/>
@@ -447,21 +446,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6B2486-83C6-437F-9C90-794FF0F55BEE}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -480,10 +480,10 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -491,10 +491,10 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -502,10 +502,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -516,7 +516,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -527,7 +527,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -535,10 +535,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -546,10 +546,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -560,7 +560,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -568,10 +568,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -579,10 +579,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -590,10 +590,10 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -601,45 +601,24 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <f>SUM(C2:C14)*0.2</f>
-        <v>1818</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+        <f>SUM(C2:C12)*0.2</f>
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C22">
+      <c r="C20">
         <f>SUM(Table2[Cost])</f>
-        <v>10908</v>
+        <v>7440</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>